<commit_message>
add source column in course excel list
</commit_message>
<xml_diff>
--- a/all_course.xlsx
+++ b/all_course.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepo\lamatxt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{824748AC-BBB8-4D58-BB72-9C63F456FBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="20331" windowHeight="8580"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="964">
   <si>
     <t>id</t>
   </si>
@@ -2903,19 +2909,17 @@
   </si>
   <si>
     <t>饮酒之过失</t>
+  </si>
+  <si>
+    <t>source</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2932,23 +2936,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2956,328 +2944,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color theme="1"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -3300,313 +2982,30 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -3891,25 +3290,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:J382"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K382"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3940,8 +3338,11 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="K1" s="2" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -3952,7 +3353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -3972,7 +3373,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -3986,7 +3387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -4000,7 +3401,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -4017,7 +3418,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -4031,7 +3432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -4042,7 +3443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -4056,7 +3457,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -4073,7 +3474,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>36</v>
       </c>
@@ -4084,7 +3485,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -4098,7 +3499,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -4118,7 +3519,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
@@ -4132,7 +3533,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -4152,7 +3553,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -4166,7 +3567,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>52</v>
       </c>
@@ -4180,7 +3581,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -4197,7 +3598,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>58</v>
       </c>
@@ -4208,7 +3609,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>60</v>
       </c>
@@ -4219,7 +3620,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>62</v>
       </c>
@@ -4230,7 +3631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>64</v>
       </c>
@@ -4241,7 +3642,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
@@ -4252,7 +3653,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>68</v>
       </c>
@@ -4263,7 +3664,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>70</v>
       </c>
@@ -4283,7 +3684,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -4300,7 +3701,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -4311,7 +3712,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -4322,7 +3723,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>82</v>
       </c>
@@ -4333,7 +3734,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>84</v>
       </c>
@@ -4344,7 +3745,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>86</v>
       </c>
@@ -4355,7 +3756,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>88</v>
       </c>
@@ -4366,7 +3767,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>90</v>
       </c>
@@ -4386,7 +3787,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>93</v>
       </c>
@@ -4397,7 +3798,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>95</v>
       </c>
@@ -4408,7 +3809,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>97</v>
       </c>
@@ -4419,7 +3820,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>99</v>
       </c>
@@ -4430,7 +3831,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>101</v>
       </c>
@@ -4450,7 +3851,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>104</v>
       </c>
@@ -4461,7 +3862,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>107</v>
       </c>
@@ -4475,7 +3876,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>110</v>
       </c>
@@ -4492,7 +3893,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>113</v>
       </c>
@@ -4506,7 +3907,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>116</v>
       </c>
@@ -4526,7 +3927,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>120</v>
       </c>
@@ -4543,7 +3944,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>122</v>
       </c>
@@ -4557,7 +3958,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>124</v>
       </c>
@@ -4571,7 +3972,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>127</v>
       </c>
@@ -4582,7 +3983,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>129</v>
       </c>
@@ -4596,7 +3997,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>131</v>
       </c>
@@ -4607,7 +4008,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>133</v>
       </c>
@@ -4621,7 +4022,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>135</v>
       </c>
@@ -4644,7 +4045,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>139</v>
       </c>
@@ -4658,7 +4059,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>141</v>
       </c>
@@ -4675,7 +4076,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>143</v>
       </c>
@@ -4689,7 +4090,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>145</v>
       </c>
@@ -4712,7 +4113,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>149</v>
       </c>
@@ -4732,7 +4133,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>152</v>
       </c>
@@ -4752,7 +4153,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>156</v>
       </c>
@@ -4766,7 +4167,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>159</v>
       </c>
@@ -4777,7 +4178,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>162</v>
       </c>
@@ -4794,7 +4195,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>165</v>
       </c>
@@ -4811,7 +4212,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>167</v>
       </c>
@@ -4828,7 +4229,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>170</v>
       </c>
@@ -4848,7 +4249,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>173</v>
       </c>
@@ -4862,7 +4263,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>176</v>
       </c>
@@ -4876,7 +4277,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>180</v>
       </c>
@@ -4890,7 +4291,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>182</v>
       </c>
@@ -4904,7 +4305,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>184</v>
       </c>
@@ -4924,7 +4325,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>188</v>
       </c>
@@ -4941,7 +4342,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>190</v>
       </c>
@@ -4961,7 +4362,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>193</v>
       </c>
@@ -4978,7 +4379,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>196</v>
       </c>
@@ -4992,7 +4393,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>198</v>
       </c>
@@ -5012,7 +4413,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>200</v>
       </c>
@@ -5032,7 +4433,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>205</v>
       </c>
@@ -5052,7 +4453,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>208</v>
       </c>
@@ -5072,7 +4473,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>211</v>
       </c>
@@ -5092,7 +4493,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>214</v>
       </c>
@@ -5112,7 +4513,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>217</v>
       </c>
@@ -5132,7 +4533,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>220</v>
       </c>
@@ -5152,7 +4553,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>223</v>
       </c>
@@ -5172,7 +4573,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>226</v>
       </c>
@@ -5192,7 +4593,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>229</v>
       </c>
@@ -5212,7 +4613,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>232</v>
       </c>
@@ -5232,7 +4633,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>235</v>
       </c>
@@ -5252,7 +4653,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>238</v>
       </c>
@@ -5272,7 +4673,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>241</v>
       </c>
@@ -5292,7 +4693,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>244</v>
       </c>
@@ -5312,7 +4713,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>247</v>
       </c>
@@ -5332,7 +4733,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>250</v>
       </c>
@@ -5352,7 +4753,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>253</v>
       </c>
@@ -5372,7 +4773,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>256</v>
       </c>
@@ -5392,7 +4793,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>259</v>
       </c>
@@ -5412,7 +4813,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>262</v>
       </c>
@@ -5432,7 +4833,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>265</v>
       </c>
@@ -5452,7 +4853,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>268</v>
       </c>
@@ -5472,7 +4873,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>271</v>
       </c>
@@ -5492,7 +4893,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>274</v>
       </c>
@@ -5512,7 +4913,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>277</v>
       </c>
@@ -5532,7 +4933,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>280</v>
       </c>
@@ -5552,7 +4953,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>283</v>
       </c>
@@ -5572,7 +4973,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>286</v>
       </c>
@@ -5592,7 +4993,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>289</v>
       </c>
@@ -5612,7 +5013,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>292</v>
       </c>
@@ -5632,7 +5033,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>295</v>
       </c>
@@ -5652,7 +5053,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="106" spans="1:5">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>298</v>
       </c>
@@ -5666,7 +5067,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>300</v>
       </c>
@@ -5686,7 +5087,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>303</v>
       </c>
@@ -5706,7 +5107,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>306</v>
       </c>
@@ -5726,7 +5127,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>309</v>
       </c>
@@ -5746,7 +5147,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="111" spans="1:5">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>312</v>
       </c>
@@ -5760,7 +5161,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="112" spans="1:5">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>314</v>
       </c>
@@ -5774,7 +5175,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="113" spans="1:5">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>316</v>
       </c>
@@ -5788,7 +5189,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="114" spans="1:5">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>318</v>
       </c>
@@ -5802,7 +5203,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="115" spans="1:5">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>320</v>
       </c>
@@ -5816,7 +5217,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="116" spans="1:5">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>322</v>
       </c>
@@ -5830,7 +5231,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="117" spans="1:5">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>324</v>
       </c>
@@ -5844,7 +5245,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="118" spans="1:5">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>326</v>
       </c>
@@ -5858,7 +5259,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="119" spans="1:5">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>328</v>
       </c>
@@ -5872,7 +5273,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="120" spans="1:5">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>330</v>
       </c>
@@ -5886,7 +5287,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>332</v>
       </c>
@@ -5900,7 +5301,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>335</v>
       </c>
@@ -5914,7 +5315,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>337</v>
       </c>
@@ -5925,7 +5326,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>339</v>
       </c>
@@ -5936,7 +5337,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>341</v>
       </c>
@@ -5947,7 +5348,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>343</v>
       </c>
@@ -5958,7 +5359,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>345</v>
       </c>
@@ -5969,7 +5370,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>347</v>
       </c>
@@ -5980,7 +5381,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>349</v>
       </c>
@@ -5991,7 +5392,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>351</v>
       </c>
@@ -6008,7 +5409,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>355</v>
       </c>
@@ -6022,7 +5423,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>357</v>
       </c>
@@ -6033,7 +5434,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>359</v>
       </c>
@@ -6053,7 +5454,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>363</v>
       </c>
@@ -6064,7 +5465,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>365</v>
       </c>
@@ -6075,7 +5476,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>367</v>
       </c>
@@ -6092,7 +5493,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>369</v>
       </c>
@@ -6103,7 +5504,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>371</v>
       </c>
@@ -6114,7 +5515,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>373</v>
       </c>
@@ -6125,7 +5526,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>375</v>
       </c>
@@ -6142,7 +5543,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="141" spans="1:3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>378</v>
       </c>
@@ -6153,7 +5554,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>380</v>
       </c>
@@ -6173,7 +5574,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>383</v>
       </c>
@@ -6190,7 +5591,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>387</v>
       </c>
@@ -6204,7 +5605,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="145" spans="1:5">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>389</v>
       </c>
@@ -6218,7 +5619,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="146" spans="1:9">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>391</v>
       </c>
@@ -6238,7 +5639,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="147" spans="1:9">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>394</v>
       </c>
@@ -6255,7 +5656,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="148" spans="1:9">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>396</v>
       </c>
@@ -6275,7 +5676,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>399</v>
       </c>
@@ -6286,7 +5687,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="150" spans="1:5">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>401</v>
       </c>
@@ -6300,7 +5701,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>403</v>
       </c>
@@ -6311,7 +5712,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>405</v>
       </c>
@@ -6328,7 +5729,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>408</v>
       </c>
@@ -6339,7 +5740,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="154" spans="1:5">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>410</v>
       </c>
@@ -6353,7 +5754,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="155" spans="1:9">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>412</v>
       </c>
@@ -6370,7 +5771,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>414</v>
       </c>
@@ -6381,7 +5782,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>416</v>
       </c>
@@ -6392,7 +5793,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>418</v>
       </c>
@@ -6403,7 +5804,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>420</v>
       </c>
@@ -6414,7 +5815,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>422</v>
       </c>
@@ -6425,7 +5826,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="161" spans="1:9">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>424</v>
       </c>
@@ -6445,7 +5846,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>427</v>
       </c>
@@ -6456,7 +5857,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>429</v>
       </c>
@@ -6467,7 +5868,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="164" spans="1:9">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>431</v>
       </c>
@@ -6481,7 +5882,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="165" spans="1:9">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>433</v>
       </c>
@@ -6498,7 +5899,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>436</v>
       </c>
@@ -6509,7 +5910,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>438</v>
       </c>
@@ -6520,7 +5921,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="168" spans="1:5">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>440</v>
       </c>
@@ -6534,7 +5935,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>443</v>
       </c>
@@ -6545,7 +5946,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>445</v>
       </c>
@@ -6556,7 +5957,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>447</v>
       </c>
@@ -6567,7 +5968,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>449</v>
       </c>
@@ -6578,7 +5979,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>451</v>
       </c>
@@ -6589,7 +5990,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>453</v>
       </c>
@@ -6600,7 +6001,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>455</v>
       </c>
@@ -6611,7 +6012,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>457</v>
       </c>
@@ -6622,7 +6023,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>459</v>
       </c>
@@ -6633,7 +6034,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>461</v>
       </c>
@@ -6644,7 +6045,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>464</v>
       </c>
@@ -6655,7 +6056,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>466</v>
       </c>
@@ -6666,7 +6067,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>468</v>
       </c>
@@ -6683,7 +6084,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="182" spans="1:5">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>470</v>
       </c>
@@ -6697,7 +6098,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="183" spans="1:5">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>473</v>
       </c>
@@ -6711,7 +6112,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>475</v>
       </c>
@@ -6722,7 +6123,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>477</v>
       </c>
@@ -6733,7 +6134,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>479</v>
       </c>
@@ -6750,7 +6151,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="187" spans="1:5">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>483</v>
       </c>
@@ -6764,7 +6165,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="188" spans="1:5">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>486</v>
       </c>
@@ -6778,7 +6179,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="189" spans="1:5">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>488</v>
       </c>
@@ -6792,7 +6193,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="190" spans="1:5">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>490</v>
       </c>
@@ -6806,7 +6207,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="191" spans="1:5">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>492</v>
       </c>
@@ -6820,7 +6221,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="192" spans="1:5">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>494</v>
       </c>
@@ -6834,7 +6235,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="193" spans="1:5">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>496</v>
       </c>
@@ -6848,7 +6249,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="194" spans="1:5">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>498</v>
       </c>
@@ -6862,7 +6263,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="195" spans="1:5">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>500</v>
       </c>
@@ -6876,7 +6277,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="196" spans="1:5">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>502</v>
       </c>
@@ -6890,7 +6291,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="197" spans="1:5">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>504</v>
       </c>
@@ -6904,7 +6305,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="198" spans="1:5">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>506</v>
       </c>
@@ -6918,7 +6319,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="199" spans="1:5">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>508</v>
       </c>
@@ -6932,7 +6333,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="200" spans="1:5">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>510</v>
       </c>
@@ -6946,7 +6347,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="201" spans="1:5">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>512</v>
       </c>
@@ -6960,7 +6361,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="202" spans="1:5">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>514</v>
       </c>
@@ -6974,7 +6375,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="203" spans="1:5">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>516</v>
       </c>
@@ -6988,7 +6389,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="204" spans="1:9">
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>519</v>
       </c>
@@ -7008,7 +6409,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="205" spans="1:7">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>522</v>
       </c>
@@ -7022,7 +6423,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>524</v>
       </c>
@@ -7033,7 +6434,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="207" spans="1:5">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>526</v>
       </c>
@@ -7047,7 +6448,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="208" spans="1:9">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>528</v>
       </c>
@@ -7061,7 +6462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="209" spans="1:5">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>530</v>
       </c>
@@ -7075,7 +6476,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="210" spans="1:5">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>532</v>
       </c>
@@ -7089,7 +6490,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="211" spans="1:9">
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>534</v>
       </c>
@@ -7103,7 +6504,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="212" spans="1:9">
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>537</v>
       </c>
@@ -7117,7 +6518,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="213" spans="1:9">
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>539</v>
       </c>
@@ -7131,7 +6532,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="214" spans="1:9">
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>541</v>
       </c>
@@ -7148,7 +6549,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="215" spans="1:9">
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>543</v>
       </c>
@@ -7162,7 +6563,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="216" spans="1:9">
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>545</v>
       </c>
@@ -7176,7 +6577,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="217" spans="1:9">
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>547</v>
       </c>
@@ -7193,7 +6594,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="218" spans="1:9">
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>549</v>
       </c>
@@ -7213,7 +6614,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="219" spans="1:9">
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>554</v>
       </c>
@@ -7233,7 +6634,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>557</v>
       </c>
@@ -7244,7 +6645,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>559</v>
       </c>
@@ -7255,7 +6656,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="222" spans="1:9">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>561</v>
       </c>
@@ -7275,7 +6676,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="223" spans="1:9">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>564</v>
       </c>
@@ -7295,7 +6696,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>567</v>
       </c>
@@ -7306,7 +6707,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="225" spans="1:9">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>569</v>
       </c>
@@ -7326,7 +6727,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="226" spans="1:9">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>572</v>
       </c>
@@ -7343,7 +6744,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="227" spans="1:9">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>575</v>
       </c>
@@ -7363,7 +6764,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="228" spans="1:5">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>579</v>
       </c>
@@ -7377,7 +6778,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="229" spans="1:5">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>581</v>
       </c>
@@ -7391,7 +6792,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="230" spans="1:9">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>583</v>
       </c>
@@ -7408,7 +6809,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="231" spans="1:9">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>586</v>
       </c>
@@ -7425,7 +6826,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="232" spans="1:9">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>590</v>
       </c>
@@ -7445,7 +6846,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="233" spans="1:9">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>593</v>
       </c>
@@ -7462,7 +6863,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="234" spans="1:9">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>596</v>
       </c>
@@ -7482,7 +6883,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="235" spans="1:9">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>599</v>
       </c>
@@ -7499,7 +6900,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="236" spans="1:9">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>602</v>
       </c>
@@ -7516,7 +6917,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>605</v>
       </c>
@@ -7527,7 +6928,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="238" spans="1:5">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>607</v>
       </c>
@@ -7541,7 +6942,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>610</v>
       </c>
@@ -7552,7 +6953,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>612</v>
       </c>
@@ -7566,7 +6967,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="241" spans="1:5">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>615</v>
       </c>
@@ -7580,7 +6981,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>617</v>
       </c>
@@ -7591,7 +6992,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="243" spans="1:9">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>619</v>
       </c>
@@ -7611,7 +7012,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>622</v>
       </c>
@@ -7622,7 +7023,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>624</v>
       </c>
@@ -7633,7 +7034,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>626</v>
       </c>
@@ -7650,7 +7051,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>629</v>
       </c>
@@ -7661,7 +7062,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="248" spans="1:9">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>631</v>
       </c>
@@ -7681,7 +7082,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="249" spans="1:5">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>634</v>
       </c>
@@ -7695,7 +7096,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>636</v>
       </c>
@@ -7706,7 +7107,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>638</v>
       </c>
@@ -7717,7 +7118,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>640</v>
       </c>
@@ -7728,7 +7129,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>642</v>
       </c>
@@ -7739,7 +7140,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>644</v>
       </c>
@@ -7750,7 +7151,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>646</v>
       </c>
@@ -7761,7 +7162,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>649</v>
       </c>
@@ -7772,7 +7173,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="257" spans="1:9">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>651</v>
       </c>
@@ -7792,7 +7193,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="258" spans="1:5">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>654</v>
       </c>
@@ -7806,7 +7207,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>656</v>
       </c>
@@ -7817,7 +7218,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="260" spans="1:9">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>658</v>
       </c>
@@ -7837,7 +7238,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="261" spans="1:9">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>661</v>
       </c>
@@ -7857,7 +7258,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="262" spans="1:5">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>664</v>
       </c>
@@ -7871,7 +7272,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="263" spans="1:5">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>666</v>
       </c>
@@ -7885,7 +7286,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="264" spans="1:5">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>669</v>
       </c>
@@ -7899,7 +7300,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>671</v>
       </c>
@@ -7913,7 +7314,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="266" spans="1:5">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>673</v>
       </c>
@@ -7927,7 +7328,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="267" spans="1:5">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>675</v>
       </c>
@@ -7941,7 +7342,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="268" spans="1:5">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>677</v>
       </c>
@@ -7955,7 +7356,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="269" spans="1:5">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>679</v>
       </c>
@@ -7969,7 +7370,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="270" spans="1:5">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>681</v>
       </c>
@@ -7983,7 +7384,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="271" spans="1:5">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>683</v>
       </c>
@@ -7997,7 +7398,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="272" spans="1:5">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>685</v>
       </c>
@@ -8011,7 +7412,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="273" spans="1:5">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>687</v>
       </c>
@@ -8025,7 +7426,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="274" spans="1:5">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>689</v>
       </c>
@@ -8039,7 +7440,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="275" spans="1:5">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>691</v>
       </c>
@@ -8053,7 +7454,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="276" spans="1:5">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>693</v>
       </c>
@@ -8067,7 +7468,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="277" spans="1:5">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>695</v>
       </c>
@@ -8081,7 +7482,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="278" spans="1:5">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>697</v>
       </c>
@@ -8095,7 +7496,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="279" spans="1:5">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>699</v>
       </c>
@@ -8109,7 +7510,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="280" spans="1:5">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>701</v>
       </c>
@@ -8123,7 +7524,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="281" spans="1:5">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>703</v>
       </c>
@@ -8137,7 +7538,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>705</v>
       </c>
@@ -8151,7 +7552,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="283" spans="1:5">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>707</v>
       </c>
@@ -8165,7 +7566,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="284" spans="1:5">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>709</v>
       </c>
@@ -8179,7 +7580,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>711</v>
       </c>
@@ -8193,7 +7594,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>713</v>
       </c>
@@ -8204,7 +7605,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="287" spans="1:5">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>715</v>
       </c>
@@ -8218,7 +7619,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>717</v>
       </c>
@@ -8232,7 +7633,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="289" spans="1:5">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>719</v>
       </c>
@@ -8246,7 +7647,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="290" spans="1:5">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>721</v>
       </c>
@@ -8260,7 +7661,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="291" spans="1:5">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>723</v>
       </c>
@@ -8274,7 +7675,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="292" spans="1:5">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>725</v>
       </c>
@@ -8288,7 +7689,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="293" spans="1:5">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>727</v>
       </c>
@@ -8302,7 +7703,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="294" spans="1:5">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>729</v>
       </c>
@@ -8316,7 +7717,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="295" spans="1:5">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>731</v>
       </c>
@@ -8330,7 +7731,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="296" spans="1:5">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>733</v>
       </c>
@@ -8344,7 +7745,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="297" spans="1:5">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>735</v>
       </c>
@@ -8358,7 +7759,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="298" spans="1:5">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>737</v>
       </c>
@@ -8372,7 +7773,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="299" spans="1:5">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>739</v>
       </c>
@@ -8386,7 +7787,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="300" spans="1:5">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>741</v>
       </c>
@@ -8400,7 +7801,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>743</v>
       </c>
@@ -8411,7 +7812,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="302" spans="1:5">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>745</v>
       </c>
@@ -8425,7 +7826,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="303" spans="1:5">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>747</v>
       </c>
@@ -8439,7 +7840,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>749</v>
       </c>
@@ -8450,7 +7851,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="305" spans="1:5">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>751</v>
       </c>
@@ -8464,7 +7865,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>753</v>
       </c>
@@ -8475,7 +7876,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>755</v>
       </c>
@@ -8486,7 +7887,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="308" spans="1:5">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>757</v>
       </c>
@@ -8500,7 +7901,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="309" spans="1:9">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>759</v>
       </c>
@@ -8514,7 +7915,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>762</v>
       </c>
@@ -8525,7 +7926,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>764</v>
       </c>
@@ -8536,7 +7937,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>766</v>
       </c>
@@ -8547,7 +7948,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>768</v>
       </c>
@@ -8558,7 +7959,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>770</v>
       </c>
@@ -8569,7 +7970,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>772</v>
       </c>
@@ -8580,7 +7981,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>774</v>
       </c>
@@ -8591,7 +7992,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="317" spans="1:5">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>776</v>
       </c>
@@ -8605,7 +8006,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>779</v>
       </c>
@@ -8616,7 +8017,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="319" spans="1:5">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>781</v>
       </c>
@@ -8630,7 +8031,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>783</v>
       </c>
@@ -8641,7 +8042,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="321" spans="1:5">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>785</v>
       </c>
@@ -8655,7 +8056,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>788</v>
       </c>
@@ -8666,7 +8067,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>790</v>
       </c>
@@ -8677,7 +8078,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="324" spans="1:8">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>792</v>
       </c>
@@ -8691,7 +8092,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="325" spans="1:9">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>796</v>
       </c>
@@ -8714,7 +8115,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="326" spans="1:8">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>800</v>
       </c>
@@ -8728,7 +8129,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>803</v>
       </c>
@@ -8742,7 +8143,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="328" spans="1:8">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>806</v>
       </c>
@@ -8759,7 +8160,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="329" spans="1:9">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>809</v>
       </c>
@@ -8782,7 +8183,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="330" spans="1:8">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>812</v>
       </c>
@@ -8796,7 +8197,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="331" spans="1:9">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>815</v>
       </c>
@@ -8819,7 +8220,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="332" spans="1:8">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>819</v>
       </c>
@@ -8836,7 +8237,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="333" spans="1:8">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>822</v>
       </c>
@@ -8850,7 +8251,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>825</v>
       </c>
@@ -8864,7 +8265,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>828</v>
       </c>
@@ -8881,7 +8282,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>832</v>
       </c>
@@ -8898,7 +8299,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>836</v>
       </c>
@@ -8915,7 +8316,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="338" spans="1:9">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>840</v>
       </c>
@@ -8938,7 +8339,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="339" spans="1:9">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>846</v>
       </c>
@@ -8958,7 +8359,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="340" spans="1:8">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>849</v>
       </c>
@@ -8972,7 +8373,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="341" spans="1:9">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>852</v>
       </c>
@@ -8995,7 +8396,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="342" spans="1:9">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>857</v>
       </c>
@@ -9018,7 +8419,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="343" spans="1:8">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>861</v>
       </c>
@@ -9032,7 +8433,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="344" spans="1:8">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>864</v>
       </c>
@@ -9049,7 +8450,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="345" spans="1:8">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>867</v>
       </c>
@@ -9063,7 +8464,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="346" spans="1:8">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>869</v>
       </c>
@@ -9077,7 +8478,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>872</v>
       </c>
@@ -9091,7 +8492,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="348" spans="1:3">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>875</v>
       </c>
@@ -9102,7 +8503,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="349" spans="1:8">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>877</v>
       </c>
@@ -9122,7 +8523,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="350" spans="1:9">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>881</v>
       </c>
@@ -9148,7 +8549,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="351" spans="1:9">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>888</v>
       </c>
@@ -9168,7 +8569,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="352" spans="1:9">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>891</v>
       </c>
@@ -9185,7 +8586,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="353" spans="1:3">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>893</v>
       </c>
@@ -9196,7 +8597,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="354" spans="1:9">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>895</v>
       </c>
@@ -9216,7 +8617,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="355" spans="1:9">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>899</v>
       </c>
@@ -9233,7 +8634,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="356" spans="1:9">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>901</v>
       </c>
@@ -9253,7 +8654,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="357" spans="1:9">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>904</v>
       </c>
@@ -9273,7 +8674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="358" spans="1:5">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>906</v>
       </c>
@@ -9287,7 +8688,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>908</v>
       </c>
@@ -9301,7 +8702,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="360" spans="1:9">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>911</v>
       </c>
@@ -9318,7 +8719,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="361" spans="1:5">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>914</v>
       </c>
@@ -9332,7 +8733,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="362" spans="1:3">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>916</v>
       </c>
@@ -9343,7 +8744,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="363" spans="1:3">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>918</v>
       </c>
@@ -9354,7 +8755,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="364" spans="1:9">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>920</v>
       </c>
@@ -9374,7 +8775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="365" spans="1:3">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>923</v>
       </c>
@@ -9385,7 +8786,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="366" spans="1:3">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>925</v>
       </c>
@@ -9396,7 +8797,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="367" spans="1:9">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>927</v>
       </c>
@@ -9413,7 +8814,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="368" spans="1:3">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>929</v>
       </c>
@@ -9424,7 +8825,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="369" spans="1:5">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>931</v>
       </c>
@@ -9438,7 +8839,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="370" spans="1:3">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>933</v>
       </c>
@@ -9449,7 +8850,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="371" spans="1:3">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>935</v>
       </c>
@@ -9460,7 +8861,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="372" spans="1:9">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>937</v>
       </c>
@@ -9477,7 +8878,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="373" spans="1:3">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>940</v>
       </c>
@@ -9488,7 +8889,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="374" spans="1:9">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>942</v>
       </c>
@@ -9502,7 +8903,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="375" spans="1:9">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>944</v>
       </c>
@@ -9516,7 +8917,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="376" spans="1:5">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>946</v>
       </c>
@@ -9530,7 +8931,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="377" spans="1:9">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>948</v>
       </c>
@@ -9553,7 +8954,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="378" spans="1:3">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>953</v>
       </c>
@@ -9564,7 +8965,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="379" spans="1:3">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>955</v>
       </c>
@@ -9575,7 +8976,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="380" spans="1:3">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>957</v>
       </c>
@@ -9586,7 +8987,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="381" spans="1:3">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>959</v>
       </c>
@@ -9597,7 +8998,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="382" spans="1:3">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>961</v>
       </c>
@@ -9609,7 +9010,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>